<commit_message>
Fixed Hamilton to work with .mhtml files
Changed:
-Fixed Hamilton to read .mhtml
-Started Montgomery

To do:
-Finish Hamilton
-Finish Montgomery
</commit_message>
<xml_diff>
--- a/Hamilton_Clerk_of_Courts_HTML_Grabber/Output/ Hamilton Midland 2023-8-6 to 2023-8-12.xlsx
+++ b/Hamilton_Clerk_of_Courts_HTML_Grabber/Output/ Hamilton Midland 2023-8-6 to 2023-8-12.xlsx
@@ -536,7 +536,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">350 CAMINO DE LA REINA STE 100 SAN DIEGO CA 92108 </t>
+          <t xml:space="preserve">350 CAMINO DE LA REINA STE 100  SAN DIEGO CA 92108 </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -546,37 +546,33 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">KLEKOTA KEVIN </t>
+          <t xml:space="preserve">BUNCE MARTIN </t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve">PO BOX 30968 MIDDLEBURG HEIGHTS OH 44130 </t>
+          <t xml:space="preserve">PO BOX 30968  MIDDLEBURG OH 44130 </t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t xml:space="preserve">96344 </t>
+          <t xml:space="preserve">79862 </t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t xml:space="preserve">ERIKA HIGGINS </t>
+          <t xml:space="preserve">ANTOINETTE GILKEY </t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t xml:space="preserve">4711 BURNET AVE CINCINNATI OH 45217 </t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">D 1 </t>
-        </is>
-      </c>
+          <t xml:space="preserve">AKA ANTOINETTE A GILKEY 1929 WASHBURN ST CINCINNATI OH 45223  </t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t xml:space="preserve">23CV17209 </t>
+          <t xml:space="preserve">23CV17210 </t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -586,7 +582,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t xml:space="preserve">MIDLAND CREDIT MANAGEMENT  INC vs. ERIKA  HIGGINS </t>
+          <t xml:space="preserve">MIDLAND CREDIT MANAGEMENT  INC vs. ANTOINETTE  GILKEY </t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -607,7 +603,7 @@
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr">
         <is>
-          <t xml:space="preserve">1912.05 </t>
+          <t xml:space="preserve">6827.23 </t>
         </is>
       </c>
       <c r="S2" t="inlineStr"/>
@@ -623,7 +619,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">350 CAMINO DE LA REINA STE 100 SAN DIEGO CA 92108 </t>
+          <t xml:space="preserve">350 CAMINO DE LA REINA STE 100  SAN DIEGO CA 92108 </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -633,27 +629,27 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">BUNCE MARTIN </t>
+          <t xml:space="preserve">PAVLOVIC NEVENKA </t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve">PO BOX 30968 MIDDLEBURG OH 44130 </t>
+          <t xml:space="preserve">PO BOX 2121  WARREN MI 48090 </t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve">79862 </t>
+          <t xml:space="preserve">72697 </t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t xml:space="preserve">ANTOINETTE GILKEY </t>
+          <t xml:space="preserve">KENARIYE DELANEY </t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t xml:space="preserve">AKA ANTOINETTE A GILKEY 1929 WASHBURN STCINCINNATI OH 45223 </t>
+          <t xml:space="preserve">1410 SPRINGFIELD PIKE APT 2  CINCINNATI OH 45215 </t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -663,7 +659,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t xml:space="preserve">23CV17210 </t>
+          <t xml:space="preserve">23CV17211 </t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -673,7 +669,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t xml:space="preserve">MIDLAND CREDIT MANAGEMENT  INC vs. ANTOINETTE  GILKEY </t>
+          <t xml:space="preserve">MIDLAND CREDIT MANAGEMENT  INC vs. KENARIYE  DELANEY </t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -694,7 +690,7 @@
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr">
         <is>
-          <t xml:space="preserve">6827.23 </t>
+          <t xml:space="preserve">1867.21 </t>
         </is>
       </c>
       <c r="S3" t="inlineStr"/>

</xml_diff>